<commit_message>
admin - import export penawaran, darah rev
</commit_message>
<xml_diff>
--- a/public/Excel/Daerah.xlsx
+++ b/public/Excel/Daerah.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\POLINEMA\SEMESTER 7\Import\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14489998-F032-462C-A743-C0FBE61A55BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A941DB9-AC54-4669-B6FD-17DE9B4BF9AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{D55AED40-25E0-4838-8453-3038A4D2BB1F}"/>
   </bookViews>
@@ -121,10 +121,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -440,10 +441,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C04914F-F436-4C06-87AF-0294C7EF62E0}">
-  <dimension ref="A1:F46"/>
+  <dimension ref="A1:H63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -452,9 +453,10 @@
     <col min="2" max="2" width="20.140625" customWidth="1"/>
     <col min="4" max="4" width="39.7109375" customWidth="1"/>
     <col min="6" max="6" width="18.28515625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -474,7 +476,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>3</v>
       </c>
@@ -488,13 +490,14 @@
         <v>2</v>
       </c>
       <c r="E2">
-        <v>2022</v>
+        <v>4</v>
       </c>
       <c r="F2" s="1">
         <v>44922</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H2" s="3"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -508,13 +511,13 @@
         <v>3</v>
       </c>
       <c r="E3">
-        <v>2022</v>
+        <v>4</v>
       </c>
       <c r="F3" s="1">
         <v>44830</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -531,7 +534,7 @@
         <v>44811</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2</v>
       </c>
@@ -540,7 +543,7 @@
       </c>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1</v>
       </c>
@@ -554,13 +557,13 @@
         <v>5</v>
       </c>
       <c r="E6">
-        <v>2022</v>
+        <v>4</v>
       </c>
       <c r="F6" s="1">
         <v>44831</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3</v>
       </c>
@@ -574,13 +577,13 @@
         <v>2</v>
       </c>
       <c r="E7">
-        <v>2022</v>
+        <v>4</v>
       </c>
       <c r="F7" s="1">
         <v>44922</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2</v>
       </c>
@@ -594,13 +597,13 @@
         <v>4</v>
       </c>
       <c r="E8">
-        <v>2022</v>
+        <v>4</v>
       </c>
       <c r="F8" s="1">
         <v>44809</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2</v>
       </c>
@@ -617,7 +620,7 @@
         <v>44810</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2</v>
       </c>
@@ -634,7 +637,7 @@
         <v>44818</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2</v>
       </c>
@@ -651,7 +654,7 @@
         <v>44816</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2</v>
       </c>
@@ -668,7 +671,7 @@
         <v>44809</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2</v>
       </c>
@@ -685,7 +688,7 @@
         <v>44816</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2</v>
       </c>
@@ -702,7 +705,7 @@
         <v>44817</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2</v>
       </c>
@@ -719,7 +722,7 @@
         <v>44812</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2</v>
       </c>
@@ -898,7 +901,7 @@
         <v>5</v>
       </c>
       <c r="E29">
-        <v>2022</v>
+        <v>4</v>
       </c>
       <c r="F29" s="1">
         <v>44840</v>
@@ -918,7 +921,7 @@
         <v>5</v>
       </c>
       <c r="E30">
-        <v>2022</v>
+        <v>4</v>
       </c>
       <c r="F30" s="1">
         <v>44825</v>
@@ -938,7 +941,7 @@
         <v>7</v>
       </c>
       <c r="E31">
-        <v>2022</v>
+        <v>4</v>
       </c>
       <c r="F31" s="1">
         <v>44825</v>
@@ -958,7 +961,7 @@
         <v>5</v>
       </c>
       <c r="E32">
-        <v>2022</v>
+        <v>4</v>
       </c>
       <c r="F32" s="1">
         <v>44826</v>
@@ -978,7 +981,7 @@
         <v>5</v>
       </c>
       <c r="E33">
-        <v>2022</v>
+        <v>4</v>
       </c>
       <c r="F33" s="1">
         <v>44830</v>
@@ -998,7 +1001,7 @@
         <v>5</v>
       </c>
       <c r="E34">
-        <v>2022</v>
+        <v>4</v>
       </c>
       <c r="F34" s="1">
         <v>44826</v>
@@ -1018,7 +1021,7 @@
         <v>5</v>
       </c>
       <c r="E35">
-        <v>2022</v>
+        <v>4</v>
       </c>
       <c r="F35" s="1">
         <v>44840</v>
@@ -1038,7 +1041,7 @@
         <v>2</v>
       </c>
       <c r="E36">
-        <v>2022</v>
+        <v>4</v>
       </c>
       <c r="F36" s="1">
         <v>44923</v>
@@ -1058,7 +1061,7 @@
         <v>2</v>
       </c>
       <c r="E37">
-        <v>2022</v>
+        <v>4</v>
       </c>
       <c r="F37" s="1">
         <v>44922</v>
@@ -1078,7 +1081,7 @@
         <v>2</v>
       </c>
       <c r="E38">
-        <v>2022</v>
+        <v>4</v>
       </c>
       <c r="F38" s="1">
         <v>44904</v>
@@ -1098,7 +1101,7 @@
         <v>2</v>
       </c>
       <c r="E39">
-        <v>2022</v>
+        <v>4</v>
       </c>
       <c r="F39" s="1">
         <v>44905</v>
@@ -1118,7 +1121,7 @@
         <v>2</v>
       </c>
       <c r="E40">
-        <v>2022</v>
+        <v>4</v>
       </c>
       <c r="F40" s="1">
         <v>44910</v>
@@ -1138,7 +1141,7 @@
         <v>2</v>
       </c>
       <c r="E41">
-        <v>2022</v>
+        <v>4</v>
       </c>
       <c r="F41" s="1">
         <v>44910</v>
@@ -1158,7 +1161,7 @@
         <v>2</v>
       </c>
       <c r="E42">
-        <v>2022</v>
+        <v>4</v>
       </c>
       <c r="F42" s="1">
         <v>44907</v>
@@ -1178,7 +1181,7 @@
         <v>2</v>
       </c>
       <c r="E43">
-        <v>2022</v>
+        <v>4</v>
       </c>
       <c r="F43" s="1">
         <v>44903</v>
@@ -1198,7 +1201,7 @@
         <v>2</v>
       </c>
       <c r="E44">
-        <v>2022</v>
+        <v>4</v>
       </c>
       <c r="F44" s="1">
         <v>44909</v>
@@ -1218,7 +1221,7 @@
         <v>2</v>
       </c>
       <c r="E45">
-        <v>2022</v>
+        <v>4</v>
       </c>
       <c r="F45" s="1">
         <v>44909</v>
@@ -1238,11 +1241,62 @@
         <v>2</v>
       </c>
       <c r="E46">
-        <v>2022</v>
+        <v>4</v>
       </c>
       <c r="F46" s="1">
         <v>44903</v>
       </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F47" s="1"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F48" s="1"/>
+    </row>
+    <row r="49" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F49" s="1"/>
+    </row>
+    <row r="50" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F50" s="1"/>
+    </row>
+    <row r="51" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F51" s="1"/>
+    </row>
+    <row r="52" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F52" s="1"/>
+    </row>
+    <row r="53" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F53" s="1"/>
+    </row>
+    <row r="54" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F54" s="1"/>
+    </row>
+    <row r="55" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F55" s="1"/>
+    </row>
+    <row r="56" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F56" s="1"/>
+    </row>
+    <row r="57" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F57" s="1"/>
+    </row>
+    <row r="58" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F58" s="1"/>
+    </row>
+    <row r="59" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F59" s="1"/>
+    </row>
+    <row r="60" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F60" s="1"/>
+    </row>
+    <row r="61" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F61" s="1"/>
+    </row>
+    <row r="62" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F62" s="1"/>
+    </row>
+    <row r="63" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F63" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>